<commit_message>
feat: update sync products from dt-one api
</commit_message>
<xml_diff>
--- a/product_fetch_report.xlsx
+++ b/product_fetch_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>Product ID</t>
   </si>
@@ -88,24 +88,99 @@
     <t>Regions</t>
   </si>
   <si>
+    <t>Roblox India 10 USD</t>
+  </si>
+  <si>
+    <t>FIXED_VALUE_PIN_PURCHASE</t>
+  </si>
+  <si>
+    <t>Get more with every Roblox Gift Card From now on, when you redeem a Roblox Gift Card, you get up to 25 more Robux. Perfect for gaming, creating, and exploring more Robux means more possibilities</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>{"base":null,"promotion_bonus":null,"total_excluding_tax":null,"total_including_tax":null}</t>
+  </si>
+  <si>
+    <t>{"id":5873,"name":"Roblox India","country":{"iso_code":"IND","name":"India","regions":[{"code":"IN-AN","name":"Andaman and Nicobar Islands"},{"code":"IND-AP","name":"Andhra Pradesh"},{"code":"IN-AR","name":"Arunachal Pradesh"},{"code":"IN-AS","name":"Assam"},{"code":"IN-BR","name":"Bihar"},{"code":"IND-BR-JH","name":"Bihar and Jharkhand"},{"code":"IN-CH","name":"Chandigarh"},{"code":"IND-TN-CN","name":"Chennai"},{"code":"IN-CT","name":"Chhattisgarh"},{"code":"IN-DH","name":"Dadra and Nagar Haveli and Daman and Diu"},{"code":"IN-DL","name":"Delhi"},{"code":"IND-DL","name":"Delhi NCR"},{"code":"IN-GA","name":"Goa"},{"code":"IND-GJ","name":"Gujarat"},{"code":"IN-HR","name":"Haryana"},{"code":"IND-HP","name":"Himachal Pradesh"},{"code":"IND","name":"India"},{"code":"IN-JK","name":"Jammu and Kashmir"},{"code":"IN-JH","name":"Jharkhand"},{"code":"IND-KA","name":"Karnataka"},{"code":"IND-KL","name":"Kerala"},{"code":"IND-WB-KK","name":"Kolkata"},{"code":"IN-LA","name":"Ladakh"},{"code":"IN-LD","name":"Lakshadweep"},{"code":"IN-MP","name":"Madhya Pradesh"},{"code":"IND-MP-CT","name":"Madhya Pradesh and Chhattisgarh"},{"code":"IN-MH","name":"Maharashtra"},{"code":"IN-MN","name":"Manipur"},{"code":"IN-ML","name":"Meghalaya"},{"code":"IN-MZ","name":"Mizoram"},{"code":"IND-MH-MB","name":"Mumbai"},{"code":"IN-NL","name":"Nagaland"},{"code":"IND-NE","name":"North East"},{"code":"IN-OR","name":"Odisha"},{"code":"IN-PY","name":"Puducherry"},{"code":"IND-PB","name":"Punjab"},{"code":"IN-RJ","name":"Rajasthan"},{"code":"IN-SK","name":"Sikkim"},{"code":"IND-TN","name":"Tamil Nadu"},{"code":"IN-TG","name":"Telangana"},{"code":"IN-TR","name":"Tripura"},{"code":"IN-UT","name":"Uttarakhand"},{"code":"IN-UP","name":"Uttar Pradesh"},{"code":"IND-UPE","name":"Uttar Pradesh East"},{"code":"IND-UPW","name":"Uttar Pradesh West"},{"code":"IN-WB","name":"West Bengal"}]},"regions":null}</t>
+  </si>
+  <si>
+    <t>{"id":4,"name":"Gift Cards","subservice":{"id":42,"name":"Gaming"}}</t>
+  </si>
+  <si>
+    <t>{"id":42,"name":"Gaming"}</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":16.33,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.612369871402327,"retail":null,"wholesale":0.612369871402327}</t>
+  </si>
+  <si>
+    <t>{"quantity":365,"unit":"DAY"}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":10,"promotion_bonus":0,"total_excluding_tax":10,"total_including_tax":10},"type":"CREDITS","unit":"USD","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>Roblox India 20 USD</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":32.65,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.612557427258806,"retail":null,"wholesale":0.612557427258806}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":20,"promotion_bonus":0,"total_excluding_tax":20,"total_including_tax":20},"type":"CREDITS","unit":"USD","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>Roblox India 50 USD</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":81.62,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.612594952217594,"retail":null,"wholesale":0.612594952217594}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":50,"promotion_bonus":0,"total_excluding_tax":50,"total_including_tax":50},"type":"CREDITS","unit":"USD","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>Roblox India 100 USD</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":163.23,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.612632481774184,"retail":null,"wholesale":0.612632481774184}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":100,"promotion_bonus":0,"total_excluding_tax":100,"total_including_tax":100},"type":"CREDITS","unit":"USD","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>Roblox India 200 USD</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":326.45,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.612651248276918,"retail":null,"wholesale":0.612651248276918}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":200,"promotion_bonus":0,"total_excluding_tax":200,"total_including_tax":200},"type":"CREDITS","unit":"USD","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
     <t>La Torre Supermercados 20 USD</t>
   </si>
   <si>
-    <t>FIXED_VALUE_PIN_PURCHASE</t>
-  </si>
-  <si>
     <t>Grocery USD 20 voucher</t>
   </si>
   <si>
-    <t>INTERNATIONAL</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>{"base":null,"promotion_bonus":null,"total_excluding_tax":null,"total_including_tax":null}</t>
-  </si>
-  <si>
     <t>{"id":2060,"name":"La Torre Supermercados Guatemala","country":{"iso_code":"GTM","name":"Guatemala","regions":[{"code":"GTM","name":"Guatemala"}]},"regions":null}</t>
   </si>
   <si>
@@ -115,7 +190,7 @@
     <t>{"id":41,"name":"Retail"}</t>
   </si>
   <si>
-    <t>{"retail":[{"Key":"amount","Value":41.99},{"Key":"fee","Value":0},{"Key":"unit","Value":"SGD"},{"Key":"unit_type","Value":"CURRENCY"}],"wholesale":{"amount":33.5867138725,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+    <t>{"retail":{"amount":41.99,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":33.5867138725,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
   </si>
   <si>
     <t>{"base":0.595473557666966,"retail":0.476303881876637,"wholesale":0.595473557666966}</t>
@@ -127,46 +202,193 @@
     <t>[{"additional_information":null,"amount":{"base":140,"promotion_bonus":0,"total_excluding_tax":140,"total_including_tax":140},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
   </si>
   <si>
-    <t>Farmacias Cruz Verde 15 USD</t>
-  </si>
-  <si>
-    <t>Pharmacy USD 15 voucher</t>
-  </si>
-  <si>
-    <t>{"id":2061,"name":"Farmacias Cruz Verde Guatemala","country":{"iso_code":"GTM","name":"Guatemala","regions":[{"code":"GTM","name":"Guatemala"}]},"regions":null}</t>
-  </si>
-  <si>
-    <t>{"retail":[{"Key":"amount","Value":31.49},{"Key":"fee","Value":0},{"Key":"unit","Value":"SGD"},{"Key":"unit_type","Value":"CURRENCY"}],"wholesale":{"amount":25.190035404375,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+    <t>La Torre Supermercados 30 USD</t>
+  </si>
+  <si>
+    <t>Grocery USD 30 voucher</t>
+  </si>
+  <si>
+    <t>{"retail":{"amount":62.98,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":50.38007080875,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
   </si>
   <si>
     <t>{"base":0.595473557666966,"retail":0.476341695776437,"wholesale":0.595473557666966}</t>
   </si>
   <si>
+    <t>[{"additional_information":null,"amount":{"base":210,"promotion_bonus":0,"total_excluding_tax":210,"total_including_tax":210},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 15 USD</t>
+  </si>
+  <si>
+    <t>Grocery USD 15 voucher</t>
+  </si>
+  <si>
+    <t>{"retail":{"amount":31.49,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":25.190035404375,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
     <t>[{"additional_information":null,"amount":{"base":105,"promotion_bonus":0,"total_excluding_tax":105,"total_including_tax":105},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
   </si>
   <si>
-    <t>Microsoft Xbox Live GiftCard Italy 25 EUR</t>
-  </si>
-  <si>
-    <t>{"id":3835,"name":"Microsoft Xbox Live Italy","country":{"iso_code":"ITA","name":"Italy","regions":[{"code":"ITA","name":"Italy"}]},"regions":null}</t>
-  </si>
-  <si>
-    <t>{"id":4,"name":"Gift Cards","subservice":{"id":42,"name":"Gaming"}}</t>
-  </si>
-  <si>
-    <t>{"id":42,"name":"Gaming"}</t>
-  </si>
-  <si>
-    <t>{"retail":null,"wholesale":{"amount":46.82,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
-  </si>
-  <si>
-    <t>{"base":0.533959846219564,"retail":null,"wholesale":0.533959846219564}</t>
-  </si>
-  <si>
-    <t>{"quantity":12,"unit":"MONTH"}</t>
-  </si>
-  <si>
-    <t>[{"additional_information":null,"amount":{"base":25,"promotion_bonus":0,"total_excluding_tax":25,"total_including_tax":25},"type":"CREDITS","unit":"EUR","unit_type":"CURRENCY"}]</t>
+    <t>La Torre Supermercados 40 USD</t>
+  </si>
+  <si>
+    <t>Grocery USD 40 voucher</t>
+  </si>
+  <si>
+    <t>{"retail":{"amount":83.97,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":67.173427745,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.595473557666966,"retail":0.476360604977968,"wholesale":0.595473557666966}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":280,"promotion_bonus":0,"total_excluding_tax":280,"total_including_tax":280},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 50 USD</t>
+  </si>
+  <si>
+    <t>Grocery USD 50 voucher</t>
+  </si>
+  <si>
+    <t>{"retail":{"amount":104.96,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":83.96678468125,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.595473557666966,"retail":0.476371951219512,"wholesale":0.595473557666966}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":350,"promotion_bonus":0,"total_excluding_tax":350,"total_including_tax":350},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 100 GTQ</t>
+  </si>
+  <si>
+    <t>Grocery 100GTQ Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":21.21,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":4.71475719000471,"retail":null,"wholesale":4.71475719000471}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":100,"promotion_bonus":0,"total_excluding_tax":100,"total_including_tax":100},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 200 GTQ</t>
+  </si>
+  <si>
+    <t>Grocery 200GTQ Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":42.42,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":200,"promotion_bonus":0,"total_excluding_tax":200,"total_including_tax":200},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 300 GTQ</t>
+  </si>
+  <si>
+    <t>Grocery 300GTQ Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":63.62,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":4.71549827098397,"retail":null,"wholesale":4.71549827098397}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":300,"promotion_bonus":0,"total_excluding_tax":300,"total_including_tax":300},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 400 GTQ</t>
+  </si>
+  <si>
+    <t>Grocery 400GTQ Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":84.83,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":4.71531297889897,"retail":null,"wholesale":4.71531297889897}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":400,"promotion_bonus":0,"total_excluding_tax":400,"total_including_tax":400},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 500 GTQ</t>
+  </si>
+  <si>
+    <t>Grocery 500GTQ Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":null,"wholesale":{"amount":106.04,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":4.7152018106375,"retail":null,"wholesale":4.7152018106375}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":500,"promotion_bonus":0,"total_excluding_tax":500,"total_including_tax":500},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 20 USD HC</t>
+  </si>
+  <si>
+    <t>Grocery 20 USD Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":{"amount":37.9,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":30.3120092699312,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.595473557666966,"retail":0.476253298153034,"wholesale":0.595473557666966}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":126.35,"promotion_bonus":0,"total_excluding_tax":126.35,"total_including_tax":126.35},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 30 USD HC</t>
+  </si>
+  <si>
+    <t>Grocery 30 USD Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":{"amount":58.89,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":47.1053662061812,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.595473557666966,"retail":0.476311767702496,"wholesale":0.595473557666966}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":196.35,"promotion_bonus":0,"total_excluding_tax":196.35,"total_including_tax":196.35},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 40 USD HC</t>
+  </si>
+  <si>
+    <t>Grocery 40 USD Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":{"amount":79.88,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":63.8987231424312,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.595473557666966,"retail":0.476339509263896,"wholesale":0.595473557666966}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":266.35,"promotion_bonus":0,"total_excluding_tax":266.35,"total_including_tax":266.35},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
+  </si>
+  <si>
+    <t>La Torre Supermercados 50 USD HC</t>
+  </si>
+  <si>
+    <t>Grocery 50 USD Voucher</t>
+  </si>
+  <si>
+    <t>{"retail":{"amount":100.87,"fee":0,"unit":"SGD","unit_type":"CURRENCY"},"wholesale":{"amount":80.6920800786812,"fee":0,"unit":"SGD","unit_type":"CURRENCY"}}</t>
+  </si>
+  <si>
+    <t>{"base":0.595473557666966,"retail":0.476355705363339,"wholesale":0.595473557666966}</t>
+  </si>
+  <si>
+    <t>[{"additional_information":null,"amount":{"base":336.35,"promotion_bonus":0,"total_excluding_tax":336.35,"total_including_tax":336.35},"type":"CREDITS","unit":"GTQ","unit_type":"CURRENCY"}]</t>
   </si>
 </sst>
 </file>
@@ -551,7 +773,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>60</v>
+        <v>59953</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -625,7 +847,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>62</v>
+        <v>59954</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
@@ -634,7 +856,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
@@ -649,7 +871,7 @@
         <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
         <v>31</v>
@@ -658,10 +880,10 @@
         <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N3" t="s">
         <v>35</v>
@@ -670,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q3" t="s">
         <v>28</v>
@@ -699,16 +921,16 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>39128</v>
+        <v>59955</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -723,51 +945,1235 @@
         <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="N4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>59956</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U5" t="s">
+        <v>28</v>
+      </c>
+      <c r="V5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W5" t="s">
+        <v>28</v>
+      </c>
+      <c r="X5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>59957</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="M6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U6" t="s">
+        <v>28</v>
+      </c>
+      <c r="V6" t="s">
+        <v>28</v>
+      </c>
+      <c r="W6" t="s">
+        <v>28</v>
+      </c>
+      <c r="X6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T7" t="s">
+        <v>28</v>
+      </c>
+      <c r="U7" t="s">
+        <v>28</v>
+      </c>
+      <c r="V7" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7" t="s">
+        <v>28</v>
+      </c>
+      <c r="X7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V8" t="s">
+        <v>28</v>
+      </c>
+      <c r="W8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" t="s">
+        <v>28</v>
+      </c>
+      <c r="U9" t="s">
+        <v>28</v>
+      </c>
+      <c r="V9" t="s">
+        <v>28</v>
+      </c>
+      <c r="W9" t="s">
+        <v>28</v>
+      </c>
+      <c r="X9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" t="s">
+        <v>73</v>
+      </c>
+      <c r="M10" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" t="s">
+        <v>28</v>
+      </c>
+      <c r="U10" t="s">
+        <v>28</v>
+      </c>
+      <c r="V10" t="s">
+        <v>28</v>
+      </c>
+      <c r="W10" t="s">
+        <v>28</v>
+      </c>
+      <c r="X10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" t="s">
+        <v>28</v>
+      </c>
+      <c r="T11" t="s">
+        <v>28</v>
+      </c>
+      <c r="U11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W11" t="s">
+        <v>28</v>
+      </c>
+      <c r="X11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" t="s">
+        <v>84</v>
+      </c>
+      <c r="N12" t="s">
+        <v>60</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" t="s">
+        <v>28</v>
+      </c>
+      <c r="V12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W12" t="s">
+        <v>28</v>
+      </c>
+      <c r="X12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>95</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" t="s">
+        <v>57</v>
+      </c>
+      <c r="L13" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" t="s">
+        <v>84</v>
+      </c>
+      <c r="N13" t="s">
+        <v>60</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S13" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" t="s">
+        <v>28</v>
+      </c>
+      <c r="U13" t="s">
+        <v>28</v>
+      </c>
+      <c r="V13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W13" t="s">
+        <v>28</v>
+      </c>
+      <c r="X13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" t="s">
+        <v>93</v>
+      </c>
+      <c r="N14" t="s">
+        <v>60</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" t="s">
+        <v>28</v>
+      </c>
+      <c r="T14" t="s">
+        <v>28</v>
+      </c>
+      <c r="U14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V14" t="s">
+        <v>28</v>
+      </c>
+      <c r="W14" t="s">
+        <v>28</v>
+      </c>
+      <c r="X14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>97</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M15" t="s">
+        <v>98</v>
+      </c>
+      <c r="N15" t="s">
+        <v>60</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" t="s">
+        <v>28</v>
+      </c>
+      <c r="U15" t="s">
+        <v>28</v>
+      </c>
+      <c r="V15" t="s">
+        <v>28</v>
+      </c>
+      <c r="W15" t="s">
+        <v>28</v>
+      </c>
+      <c r="X15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" t="s">
+        <v>103</v>
+      </c>
+      <c r="N16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>28</v>
+      </c>
+      <c r="R16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S16" t="s">
+        <v>28</v>
+      </c>
+      <c r="T16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U16" t="s">
+        <v>28</v>
+      </c>
+      <c r="V16" t="s">
+        <v>28</v>
+      </c>
+      <c r="W16" t="s">
+        <v>28</v>
+      </c>
+      <c r="X16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>128</v>
+      </c>
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" t="s">
+        <v>107</v>
+      </c>
+      <c r="M17" t="s">
+        <v>108</v>
+      </c>
+      <c r="N17" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>28</v>
+      </c>
+      <c r="R17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S17" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" t="s">
+        <v>28</v>
+      </c>
+      <c r="U17" t="s">
+        <v>28</v>
+      </c>
+      <c r="V17" t="s">
+        <v>28</v>
+      </c>
+      <c r="W17" t="s">
+        <v>28</v>
+      </c>
+      <c r="X17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>129</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" t="s">
+        <v>112</v>
+      </c>
+      <c r="M18" t="s">
+        <v>113</v>
+      </c>
+      <c r="N18" t="s">
+        <v>60</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>28</v>
+      </c>
+      <c r="R18" t="s">
+        <v>28</v>
+      </c>
+      <c r="S18" t="s">
+        <v>28</v>
+      </c>
+      <c r="T18" t="s">
+        <v>28</v>
+      </c>
+      <c r="U18" t="s">
+        <v>28</v>
+      </c>
+      <c r="V18" t="s">
+        <v>28</v>
+      </c>
+      <c r="W18" t="s">
+        <v>28</v>
+      </c>
+      <c r="X18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" t="s">
+        <v>117</v>
+      </c>
+      <c r="M19" t="s">
+        <v>118</v>
+      </c>
+      <c r="N19" t="s">
+        <v>60</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>28</v>
+      </c>
+      <c r="R19" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" t="s">
+        <v>28</v>
+      </c>
+      <c r="T19" t="s">
+        <v>28</v>
+      </c>
+      <c r="U19" t="s">
+        <v>28</v>
+      </c>
+      <c r="V19" t="s">
+        <v>28</v>
+      </c>
+      <c r="W19" t="s">
+        <v>28</v>
+      </c>
+      <c r="X19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>131</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" t="s">
+        <v>57</v>
+      </c>
+      <c r="L20" t="s">
+        <v>122</v>
+      </c>
+      <c r="M20" t="s">
+        <v>123</v>
+      </c>
+      <c r="N20" t="s">
+        <v>60</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>28</v>
+      </c>
+      <c r="R20" t="s">
+        <v>28</v>
+      </c>
+      <c r="S20" t="s">
+        <v>28</v>
+      </c>
+      <c r="T20" t="s">
+        <v>28</v>
+      </c>
+      <c r="U20" t="s">
+        <v>28</v>
+      </c>
+      <c r="V20" t="s">
+        <v>28</v>
+      </c>
+      <c r="W20" t="s">
+        <v>28</v>
+      </c>
+      <c r="X20" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>